<commit_message>
updated analysis and viz
</commit_message>
<xml_diff>
--- a/stats/hypothesis_data.xlsx
+++ b/stats/hypothesis_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Eliana/Documents/_csprojects/county-elections/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FBF6F3-9D0D-2A40-8A79-CBA80C2E868A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAA6145-9505-0A47-81A6-C438AF4C5AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14100" xr2:uid="{93E80F25-D18D-2E40-BD6F-C7FBD6FFCD95}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,7 +867,8 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L12" s="2">
-        <v>909</v>
+        <f>L3+L5-L11</f>
+        <v>926</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
fixed OTHER party not being counted issue
</commit_message>
<xml_diff>
--- a/stats/hypothesis_data.xlsx
+++ b/stats/hypothesis_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Eliana/Documents/_csprojects/county-elections/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAA6145-9505-0A47-81A6-C438AF4C5AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235144B3-1A6C-954B-8AA3-60311E9FE752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14100" xr2:uid="{93E80F25-D18D-2E40-BD6F-C7FBD6FFCD95}"/>
+    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="14100" xr2:uid="{93E80F25-D18D-2E40-BD6F-C7FBD6FFCD95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2505CED-5513-934D-B838-1C671CABD011}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="2">
-        <f>SUM(A2:K2)</f>
+        <f t="shared" ref="L2:L7" si="0">SUM(A2:K2)</f>
         <v>13</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -610,7 +610,7 @@
         <v>16</v>
       </c>
       <c r="L3" s="2">
-        <f>SUM(A3:K3)</f>
+        <f t="shared" si="0"/>
         <v>143</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -623,47 +623,47 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:K4" si="0">B3-B2</f>
+        <f t="shared" ref="B4:K4" si="1">B3-B2</f>
         <v>3</v>
       </c>
       <c r="C4" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="L4" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J4" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="K4" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L4" s="2">
-        <f>SUM(A4:K4)</f>
         <v>130</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -705,7 +705,7 @@
         <v>71</v>
       </c>
       <c r="L5" s="2">
-        <f>SUM(A5:K5)</f>
+        <f t="shared" si="0"/>
         <v>847</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -747,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(A6:K6)</f>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -755,42 +755,42 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>14</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>3</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7" s="4">
+        <v>7</v>
+      </c>
+      <c r="H7" s="4">
         <v>6</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <v>4</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <v>9</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>4</v>
       </c>
       <c r="L7" s="2">
-        <f>SUM(A7:K7)</f>
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>22</v>
@@ -799,7 +799,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L8" s="2">
         <f>L7-L2</f>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>18</v>
@@ -808,7 +808,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L9" s="2">
         <f>L5-L8</f>
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>19</v>

</xml_diff>